<commit_message>
smart merge on coordinates and readsheets
</commit_message>
<xml_diff>
--- a/data/erp/l10_gbalo.xlsx
+++ b/data/erp/l10_gbalo.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20338"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\OneDrive\Python\watex\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\repositories\watex\data\erp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{E9BDF4E5-8FF1-45F6-850C-3A3158A36749}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{547BE762-144A-4D71-8965-545E78C6217C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F3CE15-B8C3-492E-A633-F0451EC0C4BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32760" yWindow="32760" windowWidth="28800" windowHeight="12810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="16410" windowHeight="9690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="l10" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="179021"/>
 </workbook>
@@ -165,7 +165,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
+              <c:f>'l10'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -200,7 +200,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$21</c:f>
+              <c:f>'l10'!$A$2:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -269,7 +269,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$21</c:f>
+              <c:f>'l10'!$D$2:$D$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>

</xml_diff>